<commit_message>
Acabar a Task2 de modo a ter todas as Views e FE Services
</commit_message>
<xml_diff>
--- a/front-end/Task 2.xlsx
+++ b/front-end/Task 2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guicu\Documents\Universidade\Mestrado\2º Semestre\Aplicações na web\aw-project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rafae\OneDrive\Ambiente de Trabalho\MESTRADO\2 semestre\Aplicações em Web\aw-project\front-end\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{29AFA0B8-ADA2-438D-816F-79E11E102F73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1E08480-C06D-4C08-96AA-53126A7DA61C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{DF0E2589-CB8B-477F-AEE2-76A16165ADDE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DF0E2589-CB8B-477F-AEE2-76A16165ADDE}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
   <si>
     <t>Micro-frontends</t>
   </si>
@@ -36,34 +36,118 @@
     <t>Frontend Services</t>
   </si>
   <si>
-    <t>Get trending news</t>
-  </si>
-  <si>
-    <t>Get synopsis</t>
-  </si>
-  <si>
-    <t>Get full new</t>
-  </si>
-  <si>
-    <t>Get negative stats</t>
-  </si>
-  <si>
-    <t>Get positive stats</t>
-  </si>
-  <si>
-    <t>Change view to positive stats</t>
-  </si>
-  <si>
-    <t>Change view to negative stats</t>
-  </si>
-  <si>
-    <t>Read More</t>
-  </si>
-  <si>
     <t>News</t>
   </si>
   <si>
-    <t>Stats</t>
+    <t>LaunchMeatDetails</t>
+  </si>
+  <si>
+    <t>ShowProduct</t>
+  </si>
+  <si>
+    <t>ReadQRCode</t>
+  </si>
+  <si>
+    <t>LauchQRReader</t>
+  </si>
+  <si>
+    <t>ChangeViewtoNegativeStats</t>
+  </si>
+  <si>
+    <t>GetPositiveStats</t>
+  </si>
+  <si>
+    <t>ChangeViewtoPositiveStats</t>
+  </si>
+  <si>
+    <t>GetNegativeStats</t>
+  </si>
+  <si>
+    <t>GetFullNew</t>
+  </si>
+  <si>
+    <t>ReadMore</t>
+  </si>
+  <si>
+    <t>GetSynopsis</t>
+  </si>
+  <si>
+    <t>GetTrendingNews</t>
+  </si>
+  <si>
+    <t>LoadPhoto</t>
+  </si>
+  <si>
+    <t>GetMeatInfo</t>
+  </si>
+  <si>
+    <t>LaunchFeedbackPage</t>
+  </si>
+  <si>
+    <t>LoadMeatDetails</t>
+  </si>
+  <si>
+    <t>LoadSavedProd</t>
+  </si>
+  <si>
+    <t>GetFeedback</t>
+  </si>
+  <si>
+    <t>SaveProduct</t>
+  </si>
+  <si>
+    <t>LoadProductInfo</t>
+  </si>
+  <si>
+    <t>LaunchRateProdPage</t>
+  </si>
+  <si>
+    <t>SubmitFeedback</t>
+  </si>
+  <si>
+    <t>ReturnToPreviousPage</t>
+  </si>
+  <si>
+    <t>Market</t>
+  </si>
+  <si>
+    <t>Main Page</t>
+  </si>
+  <si>
+    <t>GetAvailableCategories</t>
+  </si>
+  <si>
+    <t>GetSelectedMarket</t>
+  </si>
+  <si>
+    <t>LoadMap</t>
+  </si>
+  <si>
+    <t>QR Code</t>
+  </si>
+  <si>
+    <t>LoadAvailableMarkets</t>
+  </si>
+  <si>
+    <t>GetHighlights</t>
+  </si>
+  <si>
+    <t>User Info</t>
+  </si>
+  <si>
+    <t>LoadUsersInfo</t>
+  </si>
+  <si>
+    <t>GoToSettings</t>
+  </si>
+  <si>
+    <t>GoToContacts</t>
+  </si>
+  <si>
+    <t>LogOff</t>
+  </si>
+  <si>
+    <t>GoToAccountDetails</t>
   </si>
 </sst>
 </file>
@@ -101,7 +185,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -124,22 +208,99 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -162,15 +323,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>596265</xdr:colOff>
+      <xdr:colOff>196215</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>45721</xdr:rowOff>
+      <xdr:rowOff>83821</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1346587</xdr:colOff>
+      <xdr:colOff>1609725</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>1264920</xdr:rowOff>
+      <xdr:rowOff>2380635</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -198,8 +359,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1983105" y="1706881"/>
-          <a:ext cx="750322" cy="1219199"/>
+          <a:off x="3806190" y="5160646"/>
+          <a:ext cx="1413510" cy="2296814"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -211,15 +372,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>525780</xdr:colOff>
+      <xdr:colOff>201929</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>15241</xdr:rowOff>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1316322</xdr:colOff>
+      <xdr:colOff>1571624</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>396241</xdr:rowOff>
+      <xdr:rowOff>679766</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -248,8 +409,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1912620" y="381001"/>
-          <a:ext cx="790542" cy="1318260"/>
+          <a:off x="3811904" y="2695575"/>
+          <a:ext cx="1369695" cy="2260916"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -261,15 +422,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>598170</xdr:colOff>
+      <xdr:colOff>207645</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>24434</xdr:rowOff>
+      <xdr:rowOff>81584</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1280159</xdr:colOff>
+      <xdr:colOff>1581150</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>563881</xdr:rowOff>
+      <xdr:rowOff>1118847</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -297,8 +458,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1985010" y="2996234"/>
-          <a:ext cx="681989" cy="1118567"/>
+          <a:off x="3817620" y="7568234"/>
+          <a:ext cx="1373505" cy="2237413"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -310,15 +471,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>541020</xdr:colOff>
+      <xdr:colOff>215808</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:rowOff>57149</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1264920</xdr:colOff>
+      <xdr:colOff>1543049</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>600002</xdr:rowOff>
+      <xdr:rowOff>1004900</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -347,8 +508,489 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1927860" y="4282440"/>
-          <a:ext cx="723900" cy="1171502"/>
+          <a:off x="3825783" y="9944099"/>
+          <a:ext cx="1327241" cy="2147901"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>168728</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>51707</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1638299</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>754737</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ACAC5756-E92A-C982-2C02-10AAD40E4519}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="18009" t="17800" r="19976" b="24376"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="3778703" y="12338957"/>
+          <a:ext cx="1469571" cy="2303230"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>250373</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>130628</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1590675</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>490501</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{032F7EF0-0BEC-2054-4840-EAB9F89CC00F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:srcRect l="17143" t="17976" r="19796" b="22738"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3860348" y="14818178"/>
+          <a:ext cx="1340302" cy="2160098"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>284389</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>44903</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1543050</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>1187918</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Picture 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{969955AA-5FA5-D9F0-FFA8-F9476F11BFA8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="17200" t="18900" r="19200" b="12033"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="3894364" y="17132753"/>
+          <a:ext cx="1258661" cy="2343165"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>228599</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>57149</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1685925</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>2393894</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="Picture 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{32124A5F-BE9A-4834-7A11-B0F78B28DFE5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="17391" t="18388" r="19565" b="22645"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="3838574" y="19545299"/>
+          <a:ext cx="1457326" cy="2336745"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>295273</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1647824</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>509256</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="19" name="Picture 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{83393715-80FF-758F-02C9-20CCFDD6D4CC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="18571" t="18333" r="20000" b="22500"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="3905248" y="21974175"/>
+          <a:ext cx="1352551" cy="2233281"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1314450</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>371475</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>173927</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>914401</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="20" name="Picture 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{948C9149-7FD4-93F1-90D5-9E1EEEB739E9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="3476625" y="24669750"/>
+          <a:ext cx="2126552" cy="1743076"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1647825</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>1174750</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="26" name="Picture 25">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A3A40837-62E8-A4A9-9A5C-CACA1ADE415F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="17143" t="13333" r="18571" b="24167"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="3867150" y="27012900"/>
+          <a:ext cx="1390650" cy="2317750"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>266699</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>57151</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1347439" cy="2209800"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="31" name="Picture 30">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{820B8B89-9946-48A3-BB9D-45241A079F01}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+        <a:srcRect l="18214" t="18332" r="19286" b="21876"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3876674" y="24612601"/>
+          <a:ext cx="1347439" cy="2209800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>323852</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>28576</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1628776</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>412968</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="32" name="Picture 31">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B803DF5B-D28F-3CC5-66C4-3E846D74646F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3933827" y="29384626"/>
+          <a:ext cx="1304924" cy="2289392"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -361,9 +1003,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -401,7 +1043,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -507,7 +1149,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -649,7 +1291,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -657,22 +1299,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{832E6391-5178-4AA5-93E0-67A87F0C74F9}">
-  <dimension ref="B1:D10"/>
+  <dimension ref="B1:H36"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScale="97" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A27" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.44140625" customWidth="1"/>
-    <col min="2" max="2" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.33203125" customWidth="1"/>
-    <col min="4" max="4" width="31.5546875" customWidth="1"/>
+    <col min="1" max="1" width="32.42578125" customWidth="1"/>
+    <col min="2" max="2" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.28515625" customWidth="1"/>
+    <col min="4" max="4" width="31.5703125" customWidth="1"/>
+    <col min="6" max="6" width="21.7109375" customWidth="1"/>
+    <col min="7" max="7" width="27.42578125" customWidth="1"/>
+    <col min="8" max="8" width="31.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" ht="31.8" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:4" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="2:8" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:8" ht="21" x14ac:dyDescent="0.35">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -682,74 +1327,303 @@
       <c r="D2" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="2:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="2" t="s">
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+    </row>
+    <row r="3" spans="2:8" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="9"/>
+      <c r="D3" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="17"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="15"/>
+    </row>
+    <row r="4" spans="2:8" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="7"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="17"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="15"/>
+    </row>
+    <row r="5" spans="2:8" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="7"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="17"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="15"/>
+    </row>
+    <row r="6" spans="2:8" ht="189.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="7"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="17"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="15"/>
+    </row>
+    <row r="7" spans="2:8" ht="95.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="7"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="2:4" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="2"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="4" t="s">
+      <c r="F7" s="17"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="15"/>
+    </row>
+    <row r="8" spans="2:8" ht="95.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="7"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="17"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="15"/>
+    </row>
+    <row r="9" spans="2:8" ht="95.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="7"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="17"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="15"/>
+    </row>
+    <row r="10" spans="2:8" ht="95.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="8"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10" s="17"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="15"/>
+    </row>
+    <row r="11" spans="2:8" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="9"/>
+      <c r="D11" s="14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="7"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="8"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" ht="47.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="9"/>
+      <c r="D14" s="14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" ht="47.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="7"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" ht="47.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="7"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="14" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="2:4" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="2"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="2:4" ht="103.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="2"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="2:4" ht="45.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="2:4" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="2"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="2:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="2"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="2:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="2"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="4" t="s">
-        <v>9</v>
+    <row r="17" spans="2:4" ht="47.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="7"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" ht="95.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="7"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" ht="95.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="7"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" ht="189.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="7"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="14" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" ht="47.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="7"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" ht="47.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="7"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" ht="47.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="7"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" ht="47.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="7"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" ht="95.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="7"/>
+      <c r="C25" s="12"/>
+      <c r="D25" s="14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="7"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="7"/>
+      <c r="C27" s="9"/>
+      <c r="D27" s="14" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="7"/>
+      <c r="C28" s="10"/>
+      <c r="D28" s="14" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="8"/>
+      <c r="C29" s="11"/>
+      <c r="D29" s="14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4" ht="95.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C30" s="9"/>
+      <c r="D30" s="14" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" ht="95.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="8"/>
+      <c r="C31" s="11"/>
+      <c r="D31" s="14" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4" ht="38.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C32" s="20"/>
+      <c r="D32" s="14" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" ht="38.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="3"/>
+      <c r="C33" s="20"/>
+      <c r="D33" s="14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" ht="38.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="3"/>
+      <c r="C34" s="20"/>
+      <c r="D34" s="14" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" ht="38.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="3"/>
+      <c r="C35" s="20"/>
+      <c r="D35" s="14" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" ht="38.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="3"/>
+      <c r="C36" s="20"/>
+      <c r="D36" s="14" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="B3:B6"/>
+  <mergeCells count="19">
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="B32:B36"/>
+    <mergeCell ref="C32:C36"/>
+    <mergeCell ref="F3:F10"/>
+    <mergeCell ref="G3:G5"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="C27:C29"/>
+    <mergeCell ref="B14:B29"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="C21:C24"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="C14:C17"/>
+    <mergeCell ref="C18:C19"/>
     <mergeCell ref="C3:C5"/>
-    <mergeCell ref="B7:B10"/>
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="C9:C10"/>
+    <mergeCell ref="B3:B10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>